<commit_message>
feat: excel sheet update
</commit_message>
<xml_diff>
--- a/portfolio-template.xlsx
+++ b/portfolio-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miski\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B189767D-A3D9-4332-81CF-5B4DFBDF12B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD51E07-5697-44CA-AE11-9FE9DCE4A60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{47F81816-7104-4530-86ED-67F67D81BF25}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Category</t>
   </si>
@@ -288,7 +288,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="24">
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0000000000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -360,10 +360,6 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     </dxf>
     <dxf>
@@ -418,22 +414,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8EC67BEB-09A2-4649-AC79-31F6EC22808F}" name="rec_tab" displayName="rec_tab" ref="B2:M3" totalsRowShown="0" headerRowDxfId="24">
-  <autoFilter ref="B2:M3" xr:uid="{8EC67BEB-09A2-4649-AC79-31F6EC22808F}"/>
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{F10D2F02-F4A0-4D5E-A2D1-22B117E02DCC}" name="TICKER" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{8AFB6109-EDCF-4BB0-8F02-8B3127959E48}" name="Category" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8EC67BEB-09A2-4649-AC79-31F6EC22808F}" name="rec_tab" displayName="rec_tab" ref="B2:L3" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="B2:L3" xr:uid="{8EC67BEB-09A2-4649-AC79-31F6EC22808F}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{F10D2F02-F4A0-4D5E-A2D1-22B117E02DCC}" name="TICKER" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{8AFB6109-EDCF-4BB0-8F02-8B3127959E48}" name="Category" dataDxfId="21">
       <calculatedColumnFormula>VLOOKUP(rec_tab[[#This Row],[TICKER]],tic_tab[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{9C768508-6B47-4441-AF5F-695F230480B1}" name="Broker" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{F27F0833-A525-4FAD-ABFD-36B9209CDCE9}" name="Buy Date" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{24AA9DC5-D565-4C36-AA83-F9AD1700C61A}" name="Amount" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{620A681A-6B67-4AFA-9500-FB3B84923A15}" name="Buy price" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{B1F9EF8D-950A-4E51-B35C-EE31935CE604}" name="Buy for" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{276B26DC-C3DE-4859-9927-C25CDA5830CB}" name="Sell Date" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{9B8CA652-4449-458E-A129-3CE9A7F17A2A}" name="Sell price" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{1859DD8D-486B-479A-92CF-E327D5351B6F}" name="Sell for" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{12386AF9-B9C6-4C0A-BBA7-8C913A8D615F}" name="Currency" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{9C768508-6B47-4441-AF5F-695F230480B1}" name="Broker" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{F27F0833-A525-4FAD-ABFD-36B9209CDCE9}" name="Buy Date" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{24AA9DC5-D565-4C36-AA83-F9AD1700C61A}" name="Amount" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{620A681A-6B67-4AFA-9500-FB3B84923A15}" name="Buy price" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{B1F9EF8D-950A-4E51-B35C-EE31935CE604}" name="Buy for" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{276B26DC-C3DE-4859-9927-C25CDA5830CB}" name="Sell Date" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{9B8CA652-4449-458E-A129-3CE9A7F17A2A}" name="Sell price" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{1859DD8D-486B-479A-92CF-E327D5351B6F}" name="Sell for" dataDxfId="13"/>
     <tableColumn id="12" xr3:uid="{ED6590C3-6F6C-4D98-BEF1-BA3DF092B33A}" name="Note" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -784,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AFFFC5-7AC4-42C8-9654-CCB32B0AB6A9}">
-  <dimension ref="B1:Q42"/>
+  <dimension ref="B1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,19 +797,18 @@
     <col min="9" max="9" width="16.33203125" style="7" customWidth="1"/>
     <col min="10" max="10" width="15.77734375" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.5546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="24.44140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17" customWidth="1"/>
-    <col min="16" max="16" width="15.44140625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="16.21875" customWidth="1"/>
-    <col min="18" max="18" width="14.5546875" customWidth="1"/>
+    <col min="12" max="12" width="24.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="15.44140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" customWidth="1"/>
+    <col min="17" max="17" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F1" s="4"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="2:17" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
@@ -846,13 +840,10 @@
         <v>17</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
@@ -875,57 +866,54 @@
       <c r="H3" s="10">
         <v>11540.2</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G6" s="16"/>
       <c r="H6" s="12"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G7" s="16"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G8" s="16"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G10" s="16"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G11" s="16"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G12" s="16"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G13" s="16"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G14" s="16"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G15" s="16"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
@@ -993,31 +981,31 @@
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G33" s="16"/>
       <c r="H33" s="12"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G35" s="16"/>
       <c r="H35" s="12"/>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G36" s="13"/>
       <c r="H36" s="12"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
     </row>
-    <row r="39" spans="2:16" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:15" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
@@ -1026,18 +1014,17 @@
       <c r="G39" s="13"/>
       <c r="H39" s="12"/>
       <c r="I39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="P39" s="14"/>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="O39" s="14"/>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G40" s="12"/>
       <c r="H40" s="12"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
     </row>

</xml_diff>